<commit_message>
created a separate modules config file + NLU gets conv state by DM
</commit_message>
<xml_diff>
--- a/food/resources/data_collection/NLU_for_analysis.xlsx
+++ b/food/resources/data_collection/NLU_for_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucileca/Desktop/Conversational_Agent/server_side/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucileca/Desktop/Conversational_Agent/server_side/food/resources/data_collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48693F75-ABFC-714B-80E4-91AA7303AD7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3445779-9378-6944-AB39-228593324D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NLU_for_analysis" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14001" uniqueCount="2703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14039" uniqueCount="2713">
   <si>
     <t>client_id: -LtPNkt7PDVc8m3oSxkj</t>
   </si>
@@ -8138,13 +8138,43 @@
   </si>
   <si>
     <t>missing fried chicken</t>
+  </si>
+  <si>
+    <t>Solved?</t>
+  </si>
+  <si>
+    <t>should be solved by tracking state</t>
+  </si>
+  <si>
+    <t>should be solved by adding quantifier rules</t>
+  </si>
+  <si>
+    <t>not solved but OK</t>
+  </si>
+  <si>
+    <t>create rule for thanks --&gt; yes?</t>
+  </si>
+  <si>
+    <t>not solved</t>
+  </si>
+  <si>
+    <t>solved</t>
+  </si>
+  <si>
+    <t>add failure when not understand question?</t>
+  </si>
+  <si>
+    <t>Check did not introduce more errors</t>
+  </si>
+  <si>
+    <t>?? Seems to be working now</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8275,6 +8305,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -8621,7 +8658,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
@@ -8631,6 +8668,7 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="28"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="14" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -8676,7 +8714,68 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -8989,8 +9088,8 @@
   <dimension ref="A1:M4060"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A558" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A571" sqref="A571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9974,9 +10073,6 @@
       <c r="B95" t="s">
         <v>16</v>
       </c>
-      <c r="C95" t="s">
-        <v>2683</v>
-      </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
@@ -9984,6 +10080,9 @@
       </c>
       <c r="B96" t="s">
         <v>18</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2683</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -41453,10 +41552,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF23791-306B-7B49-99AB-3E1387041D2A}">
-  <dimension ref="A1:J3054"/>
+  <dimension ref="A1:I3054"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -41464,10 +41563,10 @@
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
     <col min="2" max="2" width="61.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -41481,22 +41580,10 @@
         <v>2632</v>
       </c>
       <c r="F1" t="s">
-        <v>2633</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2634</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2635</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2654</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2655</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -41506,12 +41593,15 @@
       <c r="E2" t="s">
         <v>134</v>
       </c>
-      <c r="I2" t="s">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
+      <c r="F2" t="s">
+        <v>2704</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -41521,9 +41611,12 @@
       <c r="E3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="3" t="s">
+      <c r="F3" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>138</v>
       </c>
       <c r="B4" t="s">
@@ -41532,15 +41625,12 @@
       <c r="E4" t="s">
         <v>2661</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
+      <c r="F4" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
@@ -41549,8 +41639,11 @@
       <c r="E5" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="F5" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -41560,12 +41653,12 @@
       <c r="E6" t="s">
         <v>134</v>
       </c>
-      <c r="I6" t="s">
-        <v>2670</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5" t="s">
+      <c r="F6" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>201</v>
       </c>
       <c r="B7" t="s">
@@ -41574,9 +41667,12 @@
       <c r="E7" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
+      <c r="F7" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>213</v>
       </c>
       <c r="B8" t="s">
@@ -41585,9 +41681,12 @@
       <c r="E8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
+      <c r="F8" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
         <v>215</v>
       </c>
       <c r="B9" t="s">
@@ -41596,8 +41695,11 @@
       <c r="E9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="F9" t="s">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>218</v>
       </c>
@@ -41607,8 +41709,11 @@
       <c r="E10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="F10" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>287</v>
       </c>
@@ -41618,8 +41723,11 @@
       <c r="E11" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="F11" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -41629,8 +41737,11 @@
       <c r="E12" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="F12" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>411</v>
       </c>
@@ -41640,8 +41751,11 @@
       <c r="E13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="F13" t="s">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>435</v>
       </c>
@@ -41651,8 +41765,11 @@
       <c r="E14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="F14" t="s">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>440</v>
       </c>
@@ -41662,8 +41779,11 @@
       <c r="E15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="F15" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>454</v>
       </c>
@@ -41673,8 +41793,11 @@
       <c r="E16" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>463</v>
       </c>
@@ -41684,8 +41807,11 @@
       <c r="E17" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>464</v>
       </c>
@@ -41695,8 +41821,11 @@
       <c r="E18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>480</v>
       </c>
@@ -41706,8 +41835,11 @@
       <c r="E19" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>500</v>
       </c>
@@ -41717,8 +41849,11 @@
       <c r="E20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>528</v>
       </c>
@@ -41728,8 +41863,11 @@
       <c r="E21" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>529</v>
       </c>
@@ -41739,8 +41877,11 @@
       <c r="E22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>531</v>
       </c>
@@ -41750,8 +41891,11 @@
       <c r="E23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>534</v>
       </c>
@@ -41761,8 +41905,11 @@
       <c r="E24" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>570</v>
       </c>
@@ -41772,8 +41919,11 @@
       <c r="E25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>476</v>
       </c>
@@ -41783,8 +41933,11 @@
       <c r="E26" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>596</v>
       </c>
@@ -41794,8 +41947,11 @@
       <c r="E27" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>379</v>
       </c>
@@ -41805,9 +41961,12 @@
       <c r="E28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="7" t="s">
+      <c r="F28" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
         <v>598</v>
       </c>
       <c r="B29" t="s">
@@ -41816,8 +41975,11 @@
       <c r="E29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>605</v>
       </c>
@@ -41827,8 +41989,11 @@
       <c r="E30" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>609</v>
       </c>
@@ -41838,8 +42003,11 @@
       <c r="E31" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>629</v>
       </c>
@@ -41849,8 +42017,11 @@
       <c r="E32" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>633</v>
       </c>
@@ -41860,8 +42031,11 @@
       <c r="E33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>634</v>
       </c>
@@ -41871,8 +42045,11 @@
       <c r="E34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>653</v>
       </c>
@@ -41882,8 +42059,11 @@
       <c r="E35" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>670</v>
       </c>
@@ -41893,8 +42073,11 @@
       <c r="E36" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>672</v>
       </c>
@@ -41904,8 +42087,11 @@
       <c r="E37" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>605</v>
       </c>
@@ -41915,8 +42101,11 @@
       <c r="E38" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>379</v>
       </c>
@@ -41926,8 +42115,11 @@
       <c r="E39" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>691</v>
       </c>
@@ -41937,8 +42129,11 @@
       <c r="E40" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>700</v>
       </c>
@@ -41948,8 +42143,11 @@
       <c r="E41" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>722</v>
       </c>
@@ -41959,8 +42157,11 @@
       <c r="E42" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>724</v>
       </c>
@@ -41970,8 +42171,11 @@
       <c r="E43" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>783</v>
       </c>
@@ -41981,8 +42185,11 @@
       <c r="E44" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>809</v>
       </c>
@@ -41992,8 +42199,11 @@
       <c r="E45" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>810</v>
       </c>
@@ -42001,12 +42211,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>126</v>
       </c>
@@ -65337,6 +65547,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"not solved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"solved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"?? Seems to be working now"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>